<commit_message>
CTE Accessibility by county
</commit_message>
<xml_diff>
--- a/D4 unemployment 2021.xlsx
+++ b/D4 unemployment 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cozzieae\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C96B97-5B06-4B63-ACFC-0E5BB03E00D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF566CB-FD39-440C-9849-E5C7CD826745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20306,8 +20306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>